<commit_message>
completed task, time run 85-90 sec
</commit_message>
<xml_diff>
--- a/parse.xlsx
+++ b/parse.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,70 +356,242 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ красный</t>
+          <t>Наименование</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Код товара</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Цена</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ссылка на картинку</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ синий</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ красный</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1646107</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/853093d89e3ff3610be956c1fd95c3e2/5c126190673c5232f844241ac215a576c667e82acb9852679508270d9ae99038.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ синий</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1646102</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ зеленый</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1646104</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ серый</t>
+          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ зеленый</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1645574</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/9710105c98ee88b56ff0a7d79e1e8a05/6557ae69ab8ab3b7c6fc2918952a6d7105c54c7c0ea40dfc6b2dcaef45b1dbdb.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ фиолетовый</t>
+          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ серый</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1645572</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/06e76fe70d7e293fb5e8627c2a4bdfe8/c958b42f59f71fce27c8bbd954be0361804ce47e23933231a127f45e98cc9a9e.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ красный</t>
+          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ фиолетовый</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1645575</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3999</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/cd8dbea757059d26fc62dbc557f1b0d5/86d2c79d23d1def8eaa4ff6b126897a23d823c3c75448860d698819714df281e.png</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ синий</t>
+          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ красный</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1646114</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ фиолетовый</t>
+          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ синий</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1646112</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5399</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ фиолетовый</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1646113</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5999</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ черный</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1646108</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5999</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added run threading, time 56 sec
</commit_message>
<xml_diff>
--- a/parse.xlsx
+++ b/parse.xlsx
@@ -378,12 +378,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ красный</t>
+          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ зеленый</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1646107</t>
+          <t>1645574</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -393,19 +393,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/853093d89e3ff3610be956c1fd95c3e2/5c126190673c5232f844241ac215a576c667e82acb9852679508270d9ae99038.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/9710105c98ee88b56ff0a7d79e1e8a05/6557ae69ab8ab3b7c6fc2918952a6d7105c54c7c0ea40dfc6b2dcaef45b1dbdb.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ синий</t>
+          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ серый</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1646102</t>
+          <t>1645572</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -415,183 +415,183 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/06e76fe70d7e293fb5e8627c2a4bdfe8/c958b42f59f71fce27c8bbd954be0361804ce47e23933231a127f45e98cc9a9e.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
+          <t>6.35" Смартфон bright &amp; quick BQ 6424L MAGIC O 32 ГБ красный</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1646104</t>
+          <t>1646117</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>7450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/1223cae5f4db3cac95031a8da1ffd25d/92c5ed025c2f5179da87f639710916165f9c2fbe2e49490df61b06451e54388e.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ зеленый</t>
+          <t>5.7" Смартфон Samsung Galaxy A01 16 ГБ черный</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1645574</t>
+          <t>1623527</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>7999</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/9710105c98ee88b56ff0a7d79e1e8a05/6557ae69ab8ab3b7c6fc2918952a6d7105c54c7c0ea40dfc6b2dcaef45b1dbdb.png</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/75a04bed348bd860b23d44282764dd9a/b9a56bbadd4cf887d946ca418544bac52432f7db4878b09aaf65bc23a91b0e4b.jpg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ серый</t>
+          <t>6.52" Смартфон realme C3 64 ГБ синий</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1645572</t>
+          <t>1641173</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/06e76fe70d7e293fb5e8627c2a4bdfe8/c958b42f59f71fce27c8bbd954be0361804ce47e23933231a127f45e98cc9a9e.png</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/e4ada0fd3b6d661d68c6b977f00e4bb0/2ee2e247fef5a4be9556895a05d2af5b2bdb3b6bdd66af02192b128e18196a7b.jpg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5.99" Смартфон TP-Link Neffos A5 16 ГБ фиолетовый</t>
+          <t>6.5" Смартфон OPPO A31 64 ГБ белый</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1645575</t>
+          <t>1642439</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>11999</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/cd8dbea757059d26fc62dbc557f1b0d5/86d2c79d23d1def8eaa4ff6b126897a23d823c3c75448860d698819714df281e.png</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/afd6e1f91562be83338cd149f866811e/030a27e11b38b439b88a320f8122b836b9ec18b2de48232a1e0ef150ea491b32.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ красный</t>
+          <t>6.4" Смартфон Huawei P40 Lite 128 ГБ черный</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1646114</t>
+          <t>1640122</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>19999</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/wm/800/650/3c4e73f9c97a92b220b0453802280290/59e88fa2e38f2de590507ca98480285c6f63528cd515a481861ed9050bf40451.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ синий</t>
+          <t>6.7" Смартфон Samsung Galaxy S20+ 128 ГБ черный</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1646112</t>
+          <t>1627804</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>79999</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/53ccf05d955eb2daa680e5d5fe8e88db/1ebc2b0d87aa055e152648579180d03367ade9857a1176b8905b958971e13f3c.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ фиолетовый</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ красный</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1646113</t>
+          <t>1646107</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>3999</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/853093d89e3ff3610be956c1fd95c3e2/5c126190673c5232f844241ac215a576c667e82acb9852679508270d9ae99038.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ черный</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1646108</t>
+          <t>1646104</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>3999</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
used the library requests_html
</commit_message>
<xml_diff>
--- a/parse.xlsx
+++ b/parse.xlsx
@@ -488,110 +488,110 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6.5" Смартфон OPPO A31 64 ГБ белый</t>
+          <t>6.4" Смартфон Huawei P40 Lite 128 ГБ черный</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1642439</t>
+          <t>1640122</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11999</t>
+          <t>19999</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/afd6e1f91562be83338cd149f866811e/030a27e11b38b439b88a320f8122b836b9ec18b2de48232a1e0ef150ea491b32.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/wm/800/650/3c4e73f9c97a92b220b0453802280290/59e88fa2e38f2de590507ca98480285c6f63528cd515a481861ed9050bf40451.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6.4" Смартфон Huawei P40 Lite 128 ГБ черный</t>
+          <t>6.7" Смартфон Samsung Galaxy S20+ 128 ГБ черный</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1640122</t>
+          <t>1627804</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>19999</t>
+          <t>79999</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/wm/800/650/3c4e73f9c97a92b220b0453802280290/59e88fa2e38f2de590507ca98480285c6f63528cd515a481861ed9050bf40451.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/53ccf05d955eb2daa680e5d5fe8e88db/1ebc2b0d87aa055e152648579180d03367ade9857a1176b8905b958971e13f3c.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6.7" Смартфон Samsung Galaxy S20+ 128 ГБ черный</t>
+          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1627804</t>
+          <t>1646104</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>79999</t>
+          <t>3999</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/53ccf05d955eb2daa680e5d5fe8e88db/1ebc2b0d87aa055e152648579180d03367ade9857a1176b8905b958971e13f3c.jpg</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ красный</t>
+          <t>6.09" Смартфон bright &amp; quick BQ 6042L MAGIC E 32 ГБ фиолетовый</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1646107</t>
+          <t>1646113</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>5399</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://s.technopoint.ru/thumb/st1/fit/800/650/853093d89e3ff3610be956c1fd95c3e2/5c126190673c5232f844241ac215a576c667e82acb9852679508270d9ae99038.jpg</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/44eb27efde71257fd8cad2194c5ef83f/d82c3ec8a5cd2baccd2a464cea4a385abfc879cfbba7fb3d37d57564182fc699.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5" Смартфон bright &amp; quick BQ 5016G CHOICE 16 ГБ черный</t>
+          <t>6.15" Смартфон Honor 20 Lite 128 ГБ голубой</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1646104</t>
+          <t>1624218</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3999</t>
+          <t>14999</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>https://s.technopoint.ru/thumb/st4/fit/800/650/5680740d254a75b51c609e6ee51a88b4/51f7220e27d15d279ef679f4af9e5fa3c1f4c66bd5d722444f2ce154ac2e339b.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>